<commit_message>
tambah kode bar chart
</commit_message>
<xml_diff>
--- a/cnb/270/sentistrength-manual/stopword kecuali-no stemming/sentimen_stopword kecuali-no stemming_terpisah.xlsx
+++ b/cnb/270/sentistrength-manual/stopword kecuali-no stemming/sentimen_stopword kecuali-no stemming_terpisah.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="337">
   <si>
     <t>kecewa banget pesan free pouch dikirimnya cotton pad kaget pas unboxing untung videokan segera kabarin customer servicenya disuruh isi googleform dikirimkan ulang pouchnya hari enggak kabar akhirnya tanya dikabari kalau stock pouch ternyata habis padahal baik baik sabar mengikuti prosedur customer service berpikiran positif ternyata begini caranya</t>
   </si>
@@ -1012,6 +1012,24 @@
   </si>
   <si>
     <t>58,49%</t>
+  </si>
+  <si>
+    <t>Precision avg</t>
+  </si>
+  <si>
+    <t>51,5</t>
+  </si>
+  <si>
+    <t>Recall avg</t>
+  </si>
+  <si>
+    <t>48,32</t>
+  </si>
+  <si>
+    <t>F1 Score avg</t>
+  </si>
+  <si>
+    <t>47,19</t>
   </si>
 </sst>
 </file>
@@ -1633,10 +1651,27 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1648,13 +1683,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1663,16 +1691,6 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1997,8 +2015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K248"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F31" workbookViewId="0">
-      <selection activeCell="J56" sqref="J56"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="I59" sqref="I59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2085,13 +2103,13 @@
         <f>CHOOSE(MATCH(C4 &amp; D4, {"Negatifpositif","Negatifnetral","Negatifnegatif","Netralnegatif","Netralnetral","Netralpositif","Positifnegatif","Positifnetral","Positifpositif"}, 0), "F NegPos", "F NegNet", "T Neg", "F NetNeg", "T Net", "F NetPos", "F PosNeg", "F PosNet", "T Pos")</f>
         <v>T Neg</v>
       </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="4" t="s">
+      <c r="G4" s="7"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="11" t="s">
         <v>257</v>
       </c>
-      <c r="J4" s="5"/>
-      <c r="K4" s="6"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="13"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
@@ -2110,15 +2128,15 @@
         <f>CHOOSE(MATCH(C5 &amp; D5, {"Negatifpositif","Negatifnetral","Negatifnegatif","Netralnegatif","Netralnetral","Netralpositif","Positifnegatif","Positifnetral","Positifpositif"}, 0), "F NegPos", "F NegNet", "T Neg", "F NetNeg", "T Net", "F NetPos", "F PosNeg", "F PosNet", "T Pos")</f>
         <v>T Neg</v>
       </c>
-      <c r="G5" s="7"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="J5" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="K5" s="9" t="s">
+      <c r="G5" s="9"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2139,19 +2157,19 @@
         <f>CHOOSE(MATCH(C6 &amp; D6, {"Negatifpositif","Negatifnetral","Negatifnegatif","Netralnegatif","Netralnetral","Netralpositif","Positifnegatif","Positifnetral","Positifpositif"}, 0), "F NegPos", "F NegNet", "T Neg", "F NetNeg", "T Net", "F NetPos", "F PosNeg", "F PosNet", "T Pos")</f>
         <v>F NegPos</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="14" t="s">
         <v>258</v>
       </c>
-      <c r="H6" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="I6" s="9" t="s">
+      <c r="H6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="J6" s="9" t="s">
+      <c r="J6" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="K6" s="9" t="s">
+      <c r="K6" s="2" t="s">
         <v>250</v>
       </c>
     </row>
@@ -2172,17 +2190,17 @@
         <f>CHOOSE(MATCH(C7 &amp; D7, {"Negatifpositif","Negatifnetral","Negatifnegatif","Netralnegatif","Netralnetral","Netralpositif","Positifnegatif","Positifnetral","Positifpositif"}, 0), "F NegPos", "F NegNet", "T Neg", "F NetNeg", "T Net", "F NetPos", "F PosNeg", "F PosNet", "T Pos")</f>
         <v>T Pos</v>
       </c>
-      <c r="G7" s="11"/>
-      <c r="H7" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="I7" s="9" t="s">
+      <c r="G7" s="15"/>
+      <c r="H7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="J7" s="9" t="s">
+      <c r="J7" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="K7" s="9" t="s">
+      <c r="K7" s="2" t="s">
         <v>251</v>
       </c>
     </row>
@@ -2203,17 +2221,17 @@
         <f>CHOOSE(MATCH(C8 &amp; D8, {"Negatifpositif","Negatifnetral","Negatifnegatif","Netralnegatif","Netralnetral","Netralpositif","Positifnegatif","Positifnetral","Positifpositif"}, 0), "F NegPos", "F NegNet", "T Neg", "F NetNeg", "T Net", "F NetPos", "F PosNeg", "F PosNet", "T Pos")</f>
         <v>T Pos</v>
       </c>
-      <c r="G8" s="12"/>
-      <c r="H8" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="I8" s="9" t="s">
+      <c r="G8" s="16"/>
+      <c r="H8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="J8" s="9" t="s">
+      <c r="J8" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="K8" s="9" t="s">
+      <c r="K8" s="2" t="s">
         <v>255</v>
       </c>
     </row>
@@ -2288,13 +2306,13 @@
         <f>CHOOSE(MATCH(C12 &amp; D12, {"Negatifpositif","Negatifnetral","Negatifnegatif","Netralnegatif","Netralnetral","Netralpositif","Positifnegatif","Positifnetral","Positifpositif"}, 0), "F NegPos", "F NegNet", "T Neg", "F NetNeg", "T Net", "F NetPos", "F PosNeg", "F PosNet", "T Pos")</f>
         <v>T Pos</v>
       </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="4" t="s">
+      <c r="G12" s="7"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="11" t="s">
         <v>257</v>
       </c>
-      <c r="J12" s="5"/>
-      <c r="K12" s="6"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="13"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13">
@@ -2313,15 +2331,15 @@
         <f>CHOOSE(MATCH(C13 &amp; D13, {"Negatifpositif","Negatifnetral","Negatifnegatif","Netralnegatif","Netralnetral","Netralpositif","Positifnegatif","Positifnetral","Positifpositif"}, 0), "F NegPos", "F NegNet", "T Neg", "F NetNeg", "T Net", "F NetPos", "F PosNeg", "F PosNet", "T Pos")</f>
         <v>T Pos</v>
       </c>
-      <c r="G13" s="7"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="J13" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="K13" s="9" t="s">
+      <c r="G13" s="9"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K13" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2342,21 +2360,21 @@
         <f>CHOOSE(MATCH(C14 &amp; D14, {"Negatifpositif","Negatifnetral","Negatifnegatif","Netralnegatif","Netralnetral","Netralpositif","Positifnegatif","Positifnetral","Positifpositif"}, 0), "F NegPos", "F NegNet", "T Neg", "F NetNeg", "T Net", "F NetPos", "F PosNeg", "F PosNet", "T Pos")</f>
         <v>T Neg</v>
       </c>
-      <c r="G14" s="10" t="s">
+      <c r="G14" s="14" t="s">
         <v>258</v>
       </c>
-      <c r="H14" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="I14" s="9">
+      <c r="H14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I14" s="2">
         <f>COUNTIF(E2:E248, "T Neg") + COUNTIF(E2:E248, "T Neg ")</f>
         <v>31</v>
       </c>
-      <c r="J14" s="9">
+      <c r="J14" s="2">
         <f>COUNTIF(E2:E248, "F NegNet") + COUNTIF(E2:E248, "F NegNet ")</f>
         <v>18</v>
       </c>
-      <c r="K14" s="9">
+      <c r="K14" s="2">
         <f>COUNTIF(E2:E248, "F NegPos") + COUNTIF(E2:E248, "F NegPos ")</f>
         <v>26</v>
       </c>
@@ -2378,19 +2396,19 @@
         <f>CHOOSE(MATCH(C15 &amp; D15, {"Negatifpositif","Negatifnetral","Negatifnegatif","Netralnegatif","Netralnetral","Netralpositif","Positifnegatif","Positifnetral","Positifpositif"}, 0), "F NegPos", "F NegNet", "T Neg", "F NetNeg", "T Net", "F NetPos", "F PosNeg", "F PosNet", "T Pos")</f>
         <v>T Neg</v>
       </c>
-      <c r="G15" s="11"/>
-      <c r="H15" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="I15" s="9">
+      <c r="G15" s="15"/>
+      <c r="H15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I15" s="2">
         <f>COUNTIF(E2:E248, "F NetNeg") + COUNTIF(E2:E248, "F NetNeg ")</f>
         <v>12</v>
       </c>
-      <c r="J15" s="9">
+      <c r="J15" s="2">
         <f>COUNTIF(E2:E248, "T Net ") + COUNTIF(E2:E248, "T Net")</f>
         <v>24</v>
       </c>
-      <c r="K15" s="9">
+      <c r="K15" s="2">
         <f>COUNTIF(E2:E248, "F NetPos") + COUNTIF(E2:E248, "F NetPos ")</f>
         <v>49</v>
       </c>
@@ -2412,19 +2430,19 @@
         <f>CHOOSE(MATCH(C16 &amp; D16, {"Negatifpositif","Negatifnetral","Negatifnegatif","Netralnegatif","Netralnetral","Netralpositif","Positifnegatif","Positifnetral","Positifpositif"}, 0), "F NegPos", "F NegNet", "T Neg", "F NetNeg", "T Net", "F NetPos", "F PosNeg", "F PosNet", "T Pos")</f>
         <v>T Pos</v>
       </c>
-      <c r="G16" s="12"/>
-      <c r="H16" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="I16" s="9">
+      <c r="G16" s="16"/>
+      <c r="H16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I16" s="2">
         <f>COUNTIF(E2:E248, "F PosNeg") + COUNTIF(E2:E248, "F PosNeg ")</f>
         <v>4</v>
       </c>
-      <c r="J16" s="9">
+      <c r="J16" s="2">
         <f>COUNTIF(E2:E248, "F PosNet") + COUNTIF(E2:E248, "F PosNet ")</f>
         <v>16</v>
       </c>
-      <c r="K16" s="9">
+      <c r="K16" s="2">
         <f>COUNTIF(E2:E248, "T Pos") + COUNTIF(E2:E248, "T Pos ")</f>
         <v>67</v>
       </c>
@@ -2482,7 +2500,7 @@
         <f>CHOOSE(MATCH(C19 &amp; D19, {"Negatifpositif","Negatifnetral","Negatifnegatif","Netralnegatif","Netralnetral","Netralpositif","Positifnegatif","Positifnetral","Positifpositif"}, 0), "F NegPos", "F NegNet", "T Neg", "F NetNeg", "T Net", "F NetPos", "F PosNeg", "F PosNet", "T Pos")</f>
         <v>F NetPos</v>
       </c>
-      <c r="G19" s="13" t="s">
+      <c r="G19" s="3" t="s">
         <v>261</v>
       </c>
       <c r="H19" t="s">
@@ -2569,7 +2587,7 @@
         <f>CHOOSE(MATCH(C23 &amp; D23, {"Negatifpositif","Negatifnetral","Negatifnegatif","Netralnegatif","Netralnetral","Netralpositif","Positifnegatif","Positifnetral","Positifpositif"}, 0), "F NegPos", "F NegNet", "T Neg", "F NetNeg", "T Net", "F NetPos", "F PosNeg", "F PosNet", "T Pos")</f>
         <v>T Pos</v>
       </c>
-      <c r="H23" s="14" t="s">
+      <c r="H23" s="4" t="s">
         <v>287</v>
       </c>
     </row>
@@ -2608,7 +2626,7 @@
         <f>CHOOSE(MATCH(C25 &amp; D25, {"Negatifpositif","Negatifnetral","Negatifnegatif","Netralnegatif","Netralnetral","Netralpositif","Positifnegatif","Positifnetral","Positifpositif"}, 0), "F NegPos", "F NegNet", "T Neg", "F NetNeg", "T Net", "F NetPos", "F PosNeg", "F PosNet", "T Pos")</f>
         <v>T Neg</v>
       </c>
-      <c r="G25" s="13" t="s">
+      <c r="G25" s="3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2629,13 +2647,13 @@
         <f>CHOOSE(MATCH(C26 &amp; D26, {"Negatifpositif","Negatifnetral","Negatifnegatif","Netralnegatif","Netralnetral","Netralpositif","Positifnegatif","Positifnetral","Positifpositif"}, 0), "F NegPos", "F NegNet", "T Neg", "F NetNeg", "T Net", "F NetPos", "F PosNeg", "F PosNet", "T Pos")</f>
         <v>T Neg</v>
       </c>
-      <c r="G26" s="9" t="s">
+      <c r="G26" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="H26" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="I26" s="9" t="s">
+      <c r="H26" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I26" s="2" t="s">
         <v>264</v>
       </c>
     </row>
@@ -2656,13 +2674,13 @@
         <f>CHOOSE(MATCH(C27 &amp; D27, {"Negatifpositif","Negatifnetral","Negatifnegatif","Netralnegatif","Netralnetral","Netralpositif","Positifnegatif","Positifnetral","Positifpositif"}, 0), "F NegPos", "F NegNet", "T Neg", "F NetNeg", "T Net", "F NetPos", "F PosNeg", "F PosNet", "T Pos")</f>
         <v>F NetPos</v>
       </c>
-      <c r="G27" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="H27" s="9" t="s">
+      <c r="G27" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H27" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="I27" s="9" t="s">
+      <c r="I27" s="2" t="s">
         <v>289</v>
       </c>
     </row>
@@ -2683,13 +2701,13 @@
         <f>CHOOSE(MATCH(C28 &amp; D28, {"Negatifpositif","Negatifnetral","Negatifnegatif","Netralnegatif","Netralnetral","Netralpositif","Positifnegatif","Positifnetral","Positifpositif"}, 0), "F NegPos", "F NegNet", "T Neg", "F NetNeg", "T Net", "F NetPos", "F PosNeg", "F PosNet", "T Pos")</f>
         <v>F NegNet</v>
       </c>
-      <c r="G28" s="9" t="s">
+      <c r="G28" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="H28" s="9" t="s">
+      <c r="H28" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="I28" s="9" t="s">
+      <c r="I28" s="2" t="s">
         <v>290</v>
       </c>
     </row>
@@ -2728,7 +2746,7 @@
         <f>CHOOSE(MATCH(C30 &amp; D30, {"Negatifpositif","Negatifnetral","Negatifnegatif","Netralnegatif","Netralnetral","Netralpositif","Positifnegatif","Positifnetral","Positifpositif"}, 0), "F NegPos", "F NegNet", "T Neg", "F NetNeg", "T Net", "F NetPos", "F PosNeg", "F PosNet", "T Pos")</f>
         <v>F NegNet</v>
       </c>
-      <c r="G30" s="13" t="s">
+      <c r="G30" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2749,13 +2767,13 @@
         <f>CHOOSE(MATCH(C31 &amp; D31, {"Negatifpositif","Negatifnetral","Negatifnegatif","Netralnegatif","Netralnetral","Netralpositif","Positifnegatif","Positifnetral","Positifpositif"}, 0), "F NegPos", "F NegNet", "T Neg", "F NetNeg", "T Net", "F NetPos", "F PosNeg", "F PosNet", "T Pos")</f>
         <v>T Neg</v>
       </c>
-      <c r="G31" s="9" t="s">
+      <c r="G31" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="H31" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="I31" s="9" t="s">
+      <c r="H31" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I31" s="2" t="s">
         <v>264</v>
       </c>
     </row>
@@ -2776,13 +2794,13 @@
         <f>CHOOSE(MATCH(C32 &amp; D32, {"Negatifpositif","Negatifnetral","Negatifnegatif","Netralnegatif","Netralnetral","Netralpositif","Positifnegatif","Positifnetral","Positifpositif"}, 0), "F NegPos", "F NegNet", "T Neg", "F NetNeg", "T Net", "F NetPos", "F PosNeg", "F PosNet", "T Pos")</f>
         <v>T Pos</v>
       </c>
-      <c r="G32" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H32" s="9" t="s">
+      <c r="G32" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H32" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="I32" s="9" t="s">
+      <c r="I32" s="2" t="s">
         <v>294</v>
       </c>
     </row>
@@ -2803,13 +2821,13 @@
         <f>CHOOSE(MATCH(C33 &amp; D33, {"Negatifpositif","Negatifnetral","Negatifnegatif","Netralnegatif","Netralnetral","Netralpositif","Positifnegatif","Positifnetral","Positifpositif"}, 0), "F NegPos", "F NegNet", "T Neg", "F NetNeg", "T Net", "F NetPos", "F PosNeg", "F PosNet", "T Pos")</f>
         <v>T Net</v>
       </c>
-      <c r="G33" s="9" t="s">
+      <c r="G33" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="H33" s="9" t="s">
+      <c r="H33" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="I33" s="9" t="s">
+      <c r="I33" s="2" t="s">
         <v>293</v>
       </c>
     </row>
@@ -2848,7 +2866,7 @@
         <f>CHOOSE(MATCH(C35 &amp; D35, {"Negatifpositif","Negatifnetral","Negatifnegatif","Netralnegatif","Netralnetral","Netralpositif","Positifnegatif","Positifnetral","Positifpositif"}, 0), "F NegPos", "F NegNet", "T Neg", "F NetNeg", "T Net", "F NetPos", "F PosNeg", "F PosNet", "T Pos")</f>
         <v>T Net</v>
       </c>
-      <c r="G35" s="13" t="s">
+      <c r="G35" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2869,13 +2887,13 @@
         <f>CHOOSE(MATCH(C36 &amp; D36, {"Negatifpositif","Negatifnetral","Negatifnegatif","Netralnegatif","Netralnetral","Netralpositif","Positifnegatif","Positifnetral","Positifpositif"}, 0), "F NegPos", "F NegNet", "T Neg", "F NetNeg", "T Net", "F NetPos", "F PosNeg", "F PosNet", "T Pos")</f>
         <v>F NegPos</v>
       </c>
-      <c r="G36" s="9" t="s">
+      <c r="G36" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="H36" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="I36" s="9" t="s">
+      <c r="H36" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I36" s="2" t="s">
         <v>264</v>
       </c>
     </row>
@@ -2896,13 +2914,13 @@
         <f>CHOOSE(MATCH(C37 &amp; D37, {"Negatifpositif","Negatifnetral","Negatifnegatif","Netralnegatif","Netralnetral","Netralpositif","Positifnegatif","Positifnetral","Positifpositif"}, 0), "F NegPos", "F NegNet", "T Neg", "F NetNeg", "T Net", "F NetPos", "F PosNeg", "F PosNet", "T Pos")</f>
         <v>F NegNet</v>
       </c>
-      <c r="G37" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H37" s="9" t="s">
+      <c r="G37" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H37" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="I37" s="9" t="s">
+      <c r="I37" s="2" t="s">
         <v>297</v>
       </c>
     </row>
@@ -2923,13 +2941,13 @@
         <f>CHOOSE(MATCH(C38 &amp; D38, {"Negatifpositif","Negatifnetral","Negatifnegatif","Netralnegatif","Netralnetral","Netralpositif","Positifnegatif","Positifnetral","Positifpositif"}, 0), "F NegPos", "F NegNet", "T Neg", "F NetNeg", "T Net", "F NetPos", "F PosNeg", "F PosNet", "T Pos")</f>
         <v>F NegNet</v>
       </c>
-      <c r="G38" s="9" t="s">
+      <c r="G38" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="H38" s="9" t="s">
+      <c r="H38" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="I38" s="9" t="s">
+      <c r="I38" s="2" t="s">
         <v>298</v>
       </c>
     </row>
@@ -2968,7 +2986,7 @@
         <f>CHOOSE(MATCH(C40 &amp; D40, {"Negatifpositif","Negatifnetral","Negatifnegatif","Netralnegatif","Netralnetral","Netralpositif","Positifnegatif","Positifnetral","Positifpositif"}, 0), "F NegPos", "F NegNet", "T Neg", "F NetNeg", "T Net", "F NetPos", "F PosNeg", "F PosNet", "T Pos")</f>
         <v>T Pos</v>
       </c>
-      <c r="G40" s="13" t="s">
+      <c r="G40" s="3" t="s">
         <v>266</v>
       </c>
     </row>
@@ -2989,19 +3007,19 @@
         <f>CHOOSE(MATCH(C41 &amp; D41, {"Negatifpositif","Negatifnetral","Negatifnegatif","Netralnegatif","Netralnetral","Netralpositif","Positifnegatif","Positifnetral","Positifpositif"}, 0), "F NegPos", "F NegNet", "T Neg", "F NetNeg", "T Net", "F NetPos", "F PosNeg", "F PosNet", "T Pos")</f>
         <v>T Pos</v>
       </c>
-      <c r="G41" s="9" t="s">
+      <c r="G41" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="H41" s="15" t="s">
+      <c r="H41" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="I41" s="15" t="s">
+      <c r="I41" s="5" t="s">
         <v>269</v>
       </c>
-      <c r="J41" s="15" t="s">
+      <c r="J41" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="K41" s="15" t="s">
+      <c r="K41" s="5" t="s">
         <v>271</v>
       </c>
     </row>
@@ -3022,19 +3040,19 @@
         <f>CHOOSE(MATCH(C42 &amp; D42, {"Negatifpositif","Negatifnetral","Negatifnegatif","Netralnegatif","Netralnetral","Netralpositif","Positifnegatif","Positifnetral","Positifpositif"}, 0), "F NegPos", "F NegNet", "T Neg", "F NetNeg", "T Net", "F NetPos", "F PosNeg", "F PosNet", "T Pos")</f>
         <v>T Net</v>
       </c>
-      <c r="G42" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="H42" s="15">
+      <c r="G42" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H42" s="5">
         <v>31</v>
       </c>
-      <c r="I42" s="15">
+      <c r="I42" s="5">
         <v>16</v>
       </c>
-      <c r="J42" s="15">
+      <c r="J42" s="5">
         <v>47</v>
       </c>
-      <c r="K42" s="16"/>
+      <c r="K42" s="6"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43">
@@ -3053,19 +3071,19 @@
         <f>CHOOSE(MATCH(C43 &amp; D43, {"Negatifpositif","Negatifnetral","Negatifnegatif","Netralnegatif","Netralnetral","Netralpositif","Positifnegatif","Positifnetral","Positifpositif"}, 0), "F NegPos", "F NegNet", "T Neg", "F NetNeg", "T Net", "F NetPos", "F PosNeg", "F PosNet", "T Pos")</f>
         <v>T Pos</v>
       </c>
-      <c r="G43" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H43" s="15">
+      <c r="G43" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H43" s="5">
         <v>24</v>
       </c>
-      <c r="I43" s="15">
+      <c r="I43" s="5">
         <v>34</v>
       </c>
-      <c r="J43" s="15">
+      <c r="J43" s="5">
         <v>61</v>
       </c>
-      <c r="K43" s="16"/>
+      <c r="K43" s="6"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44">
@@ -3084,19 +3102,19 @@
         <f>CHOOSE(MATCH(C44 &amp; D44, {"Negatifpositif","Negatifnetral","Negatifnegatif","Netralnegatif","Netralnetral","Netralpositif","Positifnegatif","Positifnetral","Positifpositif"}, 0), "F NegPos", "F NegNet", "T Neg", "F NetNeg", "T Net", "F NetPos", "F PosNeg", "F PosNet", "T Pos")</f>
         <v>T Net</v>
       </c>
-      <c r="G44" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H44" s="15">
+      <c r="G44" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H44" s="5">
         <v>67</v>
       </c>
-      <c r="I44" s="15">
+      <c r="I44" s="5">
         <v>75</v>
       </c>
-      <c r="J44" s="15">
+      <c r="J44" s="5">
         <v>20</v>
       </c>
-      <c r="K44" s="16"/>
+      <c r="K44" s="6"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45">
@@ -3151,14 +3169,17 @@
         <f>CHOOSE(MATCH(C47 &amp; D47, {"Negatifpositif","Negatifnetral","Negatifnegatif","Netralnegatif","Netralnetral","Netralpositif","Positifnegatif","Positifnetral","Positifpositif"}, 0), "F NegPos", "F NegNet", "T Neg", "F NetNeg", "T Net", "F NetPos", "F PosNeg", "F PosNet", "T Pos")</f>
         <v>T Neg</v>
       </c>
-      <c r="G47" s="13" t="s">
+      <c r="G47" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="H47" s="13" t="s">
+      <c r="H47" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="I47" s="13" t="s">
+      <c r="I47" s="3" t="s">
         <v>274</v>
+      </c>
+      <c r="J47" s="3" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.3">
@@ -3188,7 +3209,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -3215,7 +3236,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
@@ -3242,7 +3263,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -3259,17 +3280,20 @@
         <f>CHOOSE(MATCH(C51 &amp; D51, {"Negatifpositif","Negatifnetral","Negatifnegatif","Netralnegatif","Netralnetral","Netralpositif","Positifnegatif","Positifnetral","Positifpositif"}, 0), "F NegPos", "F NegNet", "T Neg", "F NetNeg", "T Net", "F NetPos", "F PosNeg", "F PosNet", "T Pos")</f>
         <v>T Pos</v>
       </c>
-      <c r="G51" s="14" t="s">
+      <c r="G51" s="4" t="s">
         <v>301</v>
       </c>
-      <c r="H51" s="14" t="s">
+      <c r="H51" s="4" t="s">
         <v>304</v>
       </c>
-      <c r="I51" s="14" t="s">
+      <c r="I51" s="4" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J51" s="4" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
@@ -3287,7 +3311,7 @@
         <v>F NetNeg</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
@@ -3304,17 +3328,20 @@
         <f>CHOOSE(MATCH(C53 &amp; D53, {"Negatifpositif","Negatifnetral","Negatifnegatif","Netralnegatif","Netralnetral","Netralpositif","Positifnegatif","Positifnetral","Positifpositif"}, 0), "F NegPos", "F NegNet", "T Neg", "F NetNeg", "T Net", "F NetPos", "F PosNeg", "F PosNet", "T Pos")</f>
         <v>F NegPos</v>
       </c>
-      <c r="G53" s="13" t="s">
+      <c r="G53" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="H53" s="13" t="s">
+      <c r="H53" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="I53" s="13" t="s">
+      <c r="I53" s="3" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J53" s="3" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
@@ -3341,7 +3368,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
@@ -3368,7 +3395,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
@@ -3395,7 +3422,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
@@ -3412,17 +3439,20 @@
         <f>CHOOSE(MATCH(C57 &amp; D57, {"Negatifpositif","Negatifnetral","Negatifnegatif","Netralnegatif","Netralnetral","Netralpositif","Positifnegatif","Positifnetral","Positifpositif"}, 0), "F NegPos", "F NegNet", "T Neg", "F NetNeg", "T Net", "F NetPos", "F PosNeg", "F PosNet", "T Pos")</f>
         <v>T Neg</v>
       </c>
-      <c r="G57" s="14" t="s">
+      <c r="G57" s="4" t="s">
         <v>310</v>
       </c>
-      <c r="H57" s="14" t="s">
+      <c r="H57" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="I57" s="14">
+      <c r="I57" s="4">
         <v>0.77</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J57" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
@@ -3440,7 +3470,7 @@
         <v>F NegPos</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
@@ -3457,11 +3487,14 @@
         <f>CHOOSE(MATCH(C59 &amp; D59, {"Negatifpositif","Negatifnetral","Negatifnegatif","Netralnegatif","Netralnetral","Netralpositif","Positifnegatif","Positifnetral","Positifpositif"}, 0), "F NegPos", "F NegNet", "T Neg", "F NetNeg", "T Net", "F NetPos", "F PosNeg", "F PosNet", "T Pos")</f>
         <v>T Neg</v>
       </c>
-      <c r="G59" s="13" t="s">
+      <c r="G59" s="3" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J59" s="3" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
@@ -3482,7 +3515,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>
@@ -3503,7 +3536,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>61</v>
       </c>
@@ -3524,7 +3557,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>62</v>
       </c>
@@ -3545,7 +3578,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>63</v>
       </c>
@@ -3565,6 +3598,9 @@
       <c r="G64" t="s">
         <v>319</v>
       </c>
+      <c r="J64" t="s">
+        <v>336</v>
+      </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65">
@@ -3622,7 +3658,7 @@
         <f>CHOOSE(MATCH(C67 &amp; D67, {"Negatifpositif","Negatifnetral","Negatifnegatif","Netralnegatif","Netralnetral","Netralpositif","Positifnegatif","Positifnetral","Positifpositif"}, 0), "F NegPos", "F NegNet", "T Neg", "F NetNeg", "T Net", "F NetPos", "F PosNeg", "F PosNet", "T Pos")</f>
         <v>F PosNet</v>
       </c>
-      <c r="G67" s="13" t="s">
+      <c r="G67" s="3" t="s">
         <v>282</v>
       </c>
     </row>
@@ -3787,7 +3823,7 @@
         <f>CHOOSE(MATCH(C75 &amp; D75, {"Negatifpositif","Negatifnetral","Negatifnegatif","Netralnegatif","Netralnetral","Netralpositif","Positifnegatif","Positifnetral","Positifpositif"}, 0), "F NegPos", "F NegNet", "T Neg", "F NetNeg", "T Net", "F NetPos", "F PosNeg", "F PosNet", "T Pos")</f>
         <v>T Pos</v>
       </c>
-      <c r="G75" s="13" t="s">
+      <c r="G75" s="3" t="s">
         <v>283</v>
       </c>
     </row>
@@ -3913,7 +3949,7 @@
         <f>CHOOSE(MATCH(C81 &amp; D81, {"Negatifpositif","Negatifnetral","Negatifnegatif","Netralnegatif","Netralnetral","Netralpositif","Positifnegatif","Positifnetral","Positifpositif"}, 0), "F NegPos", "F NegNet", "T Neg", "F NetNeg", "T Net", "F NetPos", "F PosNeg", "F PosNet", "T Pos")</f>
         <v>F NegNet</v>
       </c>
-      <c r="G81" s="14" t="s">
+      <c r="G81" s="4" t="s">
         <v>330</v>
       </c>
     </row>
@@ -6925,13 +6961,14 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="G14:G16"/>
     <mergeCell ref="G4:H5"/>
     <mergeCell ref="I4:K4"/>
     <mergeCell ref="G6:G8"/>
     <mergeCell ref="G12:H13"/>
     <mergeCell ref="I12:K12"/>
-    <mergeCell ref="G14:G16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>